<commit_message>
create pure ascii version of Jenkins spreadsheet
this was added as Jenkins09_ISM_Tab4.txt
</commit_message>
<xml_diff>
--- a/data/abundances/Jenkins09_ISM_Tab4.xlsx
+++ b/data/abundances/Jenkins09_ISM_Tab4.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chama\Google Drive\[O I] Research w. Ferland, Renbin, &amp; Xihan Ji\Depletion Factor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/cloudy/branches/jenkins09/data/abundances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB3B283-F37F-440F-A410-2A8373F6C309}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277BB9E4-B32C-D240-AA0F-6AFF1D82A5B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="624" windowWidth="17772" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26940" yWindow="9320" windowWidth="17780" windowHeight="12340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -187,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>C</t>
   </si>
@@ -393,6 +394,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Courier"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3681,40 +3683,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScale="95" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="6" width="7.796875" customWidth="1"/>
-    <col min="7" max="7" width="13.296875" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="20" width="13.296875" customWidth="1"/>
+    <col min="4" max="6" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="20" width="13.33203125" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.69921875" customWidth="1"/>
-    <col min="23" max="23" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" customWidth="1"/>
-    <col min="36" max="36" width="4.69921875" customWidth="1"/>
-    <col min="37" max="37" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.6640625" customWidth="1"/>
+    <col min="37" max="37" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -3824,7 +3826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3968,7 @@
       </c>
       <c r="AL2" s="14"/>
     </row>
-    <row r="3" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -4108,7 +4110,7 @@
       </c>
       <c r="AL3" s="24"/>
     </row>
-    <row r="4" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
@@ -4250,7 +4252,7 @@
       </c>
       <c r="AL4" s="25"/>
     </row>
-    <row r="5" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -4392,7 +4394,7 @@
       </c>
       <c r="AL5" s="16"/>
     </row>
-    <row r="6" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
@@ -4534,7 +4536,7 @@
       </c>
       <c r="AL6" s="16"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -4676,7 +4678,7 @@
       </c>
       <c r="AL7" s="14"/>
     </row>
-    <row r="8" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
@@ -4818,7 +4820,7 @@
       </c>
       <c r="AL8" s="25"/>
     </row>
-    <row r="9" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -4960,7 +4962,7 @@
       </c>
       <c r="AL9" s="14"/>
     </row>
-    <row r="10" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
@@ -5102,7 +5104,7 @@
       </c>
       <c r="AL10" s="14"/>
     </row>
-    <row r="11" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -5244,7 +5246,7 @@
       </c>
       <c r="AL11" s="14"/>
     </row>
-    <row r="12" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
@@ -5386,7 +5388,7 @@
       </c>
       <c r="AL12" s="14"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
@@ -5528,7 +5530,7 @@
       </c>
       <c r="AL13" s="14"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -5670,7 +5672,7 @@
       </c>
       <c r="AL14" s="14"/>
     </row>
-    <row r="15" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
@@ -5812,7 +5814,7 @@
       </c>
       <c r="AL15" s="14"/>
     </row>
-    <row r="16" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
@@ -5954,7 +5956,7 @@
       </c>
       <c r="AL16" s="14"/>
     </row>
-    <row r="17" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -6096,7 +6098,7 @@
       </c>
       <c r="AL17" s="14"/>
     </row>
-    <row r="18" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
@@ -6238,7 +6240,7 @@
       </c>
       <c r="AL18" s="14"/>
     </row>
-    <row r="19" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="C19" s="6"/>
       <c r="D19" s="13"/>
@@ -6276,7 +6278,7 @@
       <c r="AK19" s="43"/>
       <c r="AL19" s="43"/>
     </row>
-    <row r="20" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="C20" s="38"/>
       <c r="D20" s="39"/>
@@ -6314,7 +6316,7 @@
       <c r="AK20" s="41"/>
       <c r="AL20" s="41"/>
     </row>
-    <row r="21" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="C21" s="38"/>
       <c r="D21" s="39"/>
@@ -6352,7 +6354,7 @@
       <c r="AK21" s="41"/>
       <c r="AL21" s="41"/>
     </row>
-    <row r="22" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="C22" s="38"/>
       <c r="D22" s="39"/>
@@ -6390,7 +6392,7 @@
       <c r="AK22" s="41"/>
       <c r="AL22" s="41"/>
     </row>
-    <row r="23" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="C23" s="38"/>
       <c r="D23" s="39"/>
@@ -6428,7 +6430,7 @@
       <c r="AK23" s="41"/>
       <c r="AL23" s="41"/>
     </row>
-    <row r="24" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="C24" s="38"/>
       <c r="D24" s="39"/>
@@ -6466,7 +6468,7 @@
       <c r="AK24" s="41"/>
       <c r="AL24" s="41"/>
     </row>
-    <row r="25" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="C25" s="38"/>
       <c r="D25" s="39"/>
@@ -6504,7 +6506,7 @@
       <c r="AK25" s="41"/>
       <c r="AL25" s="41"/>
     </row>
-    <row r="26" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="C26" s="38"/>
       <c r="D26" s="13"/>
@@ -6542,7 +6544,7 @@
       <c r="AK26" s="41"/>
       <c r="AL26" s="41"/>
     </row>
-    <row r="27" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="C27" s="38"/>
       <c r="D27" s="13"/>
@@ -6580,7 +6582,7 @@
       <c r="AK27" s="41"/>
       <c r="AL27" s="41"/>
     </row>
-    <row r="28" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="C28" s="6"/>
       <c r="D28" s="13"/>
@@ -6608,7 +6610,7 @@
       <c r="AK28" s="43"/>
       <c r="AL28" s="43"/>
     </row>
-    <row r="29" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="C29" s="38"/>
       <c r="D29" s="13"/>
@@ -6646,7 +6648,7 @@
       <c r="AK29" s="41"/>
       <c r="AL29" s="41"/>
     </row>
-    <row r="30" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="C30" s="6"/>
       <c r="D30" s="13"/>
@@ -6674,7 +6676,7 @@
       <c r="AK30" s="43"/>
       <c r="AL30" s="43"/>
     </row>
-    <row r="31" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="C31" s="6"/>
       <c r="D31" s="13"/>
@@ -6742,7 +6744,7 @@
       <c r="AK31" s="43"/>
       <c r="AL31" s="43"/>
     </row>
-    <row r="32" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="C32" s="6"/>
       <c r="D32" s="13"/>
@@ -6780,7 +6782,7 @@
       <c r="AK32" s="43"/>
       <c r="AL32" s="43"/>
     </row>
-    <row r="33" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="C33" s="6"/>
       <c r="D33" s="13"/>
@@ -6818,7 +6820,7 @@
       <c r="AK33" s="43"/>
       <c r="AL33" s="43"/>
     </row>
-    <row r="34" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="C34" s="6"/>
       <c r="D34" s="13"/>
@@ -6856,7 +6858,7 @@
       <c r="AK34" s="43"/>
       <c r="AL34" s="43"/>
     </row>
-    <row r="35" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="C35" s="6"/>
       <c r="D35" s="13"/>
@@ -6894,7 +6896,7 @@
       <c r="AK35" s="43"/>
       <c r="AL35" s="43"/>
     </row>
-    <row r="36" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="C36" s="6"/>
       <c r="D36" s="13"/>
@@ -6932,7 +6934,7 @@
       <c r="AK36" s="43"/>
       <c r="AL36" s="43"/>
     </row>
-    <row r="37" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="C37" s="6"/>
       <c r="D37" s="13"/>
@@ -6970,7 +6972,7 @@
       <c r="AK37" s="43"/>
       <c r="AL37" s="43"/>
     </row>
-    <row r="38" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="C38" s="6"/>
       <c r="D38" s="13"/>
@@ -7008,7 +7010,7 @@
       <c r="AK38" s="43"/>
       <c r="AL38" s="43"/>
     </row>
-    <row r="39" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="C39" s="6"/>
       <c r="D39" s="13"/>
@@ -7046,16 +7048,16 @@
       <c r="AK39" s="43"/>
       <c r="AL39" s="43"/>
     </row>
-    <row r="40" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="37"/>
     </row>
-    <row r="41" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="37"/>
     </row>
-    <row r="42" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="37"/>
     </row>
-    <row r="43" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="37"/>
     </row>
   </sheetData>
@@ -7070,4 +7072,425 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2E191B-0B02-2C4E-9847-A4CEC7C39A25}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>-0.193</v>
+      </c>
+      <c r="C2" s="12">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-0.109</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28">
+        <v>-0.14499999999999999</v>
+      </c>
+      <c r="C4" s="28">
+        <v>-0.22500000000000001</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="32">
+        <v>-0.8</v>
+      </c>
+      <c r="C5" s="32">
+        <v>-0.997</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="32">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="C6" s="32">
+        <v>-1.1359999999999999</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12">
+        <v>-0.16600000000000001</v>
+      </c>
+      <c r="C7" s="12">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="28">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="C8" s="28">
+        <v>-0.879</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13">
+        <v>-0.314</v>
+      </c>
+      <c r="C9" s="13">
+        <v>-1.242</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>-1.9570000000000001</v>
+      </c>
+      <c r="C10" s="13">
+        <v>-2.048</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <v>-1.508</v>
+      </c>
+      <c r="C11" s="13">
+        <v>-1.4470000000000001</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <v>-1.3540000000000001</v>
+      </c>
+      <c r="C12" s="13">
+        <v>-0.85699999999999998</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12">
+        <v>-1.5129999999999999</v>
+      </c>
+      <c r="C13" s="12">
+        <v>-1.2849999999999999</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="12">
+        <v>-1.829</v>
+      </c>
+      <c r="C14" s="12">
+        <v>-1.49</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.59899999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="13">
+        <v>-1.1020000000000001</v>
+      </c>
+      <c r="C15" s="13">
+        <v>-0.71</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13">
+        <v>-0.27900000000000003</v>
+      </c>
+      <c r="C16" s="13">
+        <v>-0.61</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="13">
+        <v>-0.72499999999999998</v>
+      </c>
+      <c r="C17" s="13">
+        <v>-0.61499999999999999</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="13">
+        <v>-0.33200000000000002</v>
+      </c>
+      <c r="C18" s="13">
+        <v>-0.16600000000000001</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="10"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="10"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="37"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="37"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="37"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>